<commit_message>
cross browser and parallel implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/testdata.xlsx
+++ b/src/test/resources/TestData/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\02199\eclipse-workspace\DSAlgo\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163013F6-1734-44A8-9CB9-F04E9DF75B05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3C403D-B6BC-4C6C-B37D-99774C2749B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="20" windowWidth="22540" windowHeight="14300" xr2:uid="{96C06443-7610-4BC9-9E10-3D39FD2144DD}"/>
   </bookViews>
@@ -25,7 +25,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
   <si>
     <t>Element Found</t>
   </si>
@@ -109,13 +118,37 @@
     <t>print("Hello")</t>
   </si>
   <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>output</t>
-  </si>
-  <si>
-    <t>hello</t>
+    <t>TestName</t>
+  </si>
+  <si>
+    <t>Print valid Hello</t>
+  </si>
+  <si>
+    <t>Print invalid Hello</t>
+  </si>
+  <si>
+    <t>Run Search Practice</t>
+  </si>
+  <si>
+    <t>Submit Search Practice</t>
+  </si>
+  <si>
+    <t>Run findMaxConsecutiveOnes Practice</t>
+  </si>
+  <si>
+    <t>Run findNumbers Practice</t>
+  </si>
+  <si>
+    <t>Submit findNumbers Practice</t>
+  </si>
+  <si>
+    <t>Run sortedSquares Practice</t>
+  </si>
+  <si>
+    <t>Submit sortedSquares Practice</t>
+  </si>
+  <si>
+    <t>Submit findMaxConsecutiveOnes Practice</t>
   </si>
 </sst>
 </file>
@@ -164,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -187,22 +220,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -211,10 +233,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,111 +548,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9429FDAC-9F73-44C8-B623-9BE65DFF2AC9}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="148.36328125" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.36328125" customWidth="1"/>
+    <col min="2" max="2" width="195.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>